<commit_message>
top / side / bottom 분리
</commit_message>
<xml_diff>
--- a/설계/포커스리더 프로젝트 매니저 DB설계V_05.xlsx
+++ b/설계/포커스리더 프로젝트 매니저 DB설계V_05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a287e4f135fd79b0/문서/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djrl0\IdeaProjects\FLPJTMGR22\설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{77F9FB3B-3694-4E8F-AE35-F28D08F03252}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E05BF13-4C1A-4FF4-8FBB-400A9A3409D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16459A8-1CC9-4D02-BFD2-95E78ED6D31E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FD4732AD-A8E9-4B40-97D9-1D21EEA29345}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="2" xr2:uid="{FD4732AD-A8E9-4B40-97D9-1D21EEA29345}"/>
   </bookViews>
   <sheets>
     <sheet name="공통코드 테이블" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="133">
   <si>
     <t>프로젝트명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1253,6 +1253,15 @@
     <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1291,15 +1300,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1636,7 +1636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755DA47-7F91-4AA0-841E-2FE0E7ECEC29}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1657,16 +1657,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -1675,15 +1675,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -1692,44 +1692,44 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="62" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="51" t="s">
@@ -1847,7 +1847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EAF6CC-F066-4611-85AE-56D407ABC086}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1868,16 +1868,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -1886,15 +1886,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -1903,44 +1903,44 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="27">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2059,16 +2059,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -2077,15 +2077,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -2094,44 +2094,44 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
@@ -2160,7 +2160,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="13.5">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="62" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -2238,9 +2238,7 @@
       <c r="B10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="42" t="s">
-        <v>23</v>
-      </c>
+      <c r="C10" s="42"/>
       <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
@@ -2275,7 +2273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC5EAB2-DADE-41E9-ACFA-9FC4AF766C00}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2296,16 +2294,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -2314,15 +2312,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -2331,59 +2329,59 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2625,7 +2623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18931DC6-D2E8-4E59-846A-14FB790C9A06}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2646,16 +2644,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -2664,15 +2662,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -2681,59 +2679,59 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2972,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD8CE3D-BEFE-4BB1-BEB7-EFB1EDD585E6}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2993,16 +2991,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -3011,15 +3009,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -3028,59 +3026,59 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3324,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ADC51C8-2D1F-423D-B730-F3E91284B20C}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3345,16 +3343,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
@@ -3363,15 +3361,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="70">
         <v>44211</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -3380,59 +3378,59 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="G3" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3592,7 +3590,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="13.5">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="61" t="s">
         <v>94</v>
       </c>
       <c r="B14" s="8" t="s">

</xml_diff>